<commit_message>
Update manuals and Program
</commit_message>
<xml_diff>
--- a/test/calibration.xlsx
+++ b/test/calibration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\PlatformIO\Projects\Lambda Shifter OTA\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B65F56CF-CF48-48B3-B036-D133CFB4E87B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEB88498-04F8-4E1B-A8FC-657C871530A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12825" yWindow="120" windowWidth="12945" windowHeight="12570" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="61">
   <si>
     <r>
       <t>200mV</t>
@@ -450,6 +450,33 @@
     <t>LS20-AP0023 #2</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>LS20-AP0027 #2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>LS20-AP003１#1</t>
+  </si>
+  <si>
+    <t>LS20-AP003１#1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>LS20-AP0032#1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>LS20-AP0033</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>LS20-AP0034#2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>LS20-AP0034#1</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
@@ -657,7 +684,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -740,6 +767,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -779,22 +812,10 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1083,7 +1104,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A45" sqref="A45"/>
+      <selection pane="bottomLeft" activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1100,30 +1121,30 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="18.75" x14ac:dyDescent="0.4">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="33" t="s">
+      <c r="D2" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="34"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="33" t="s">
+      <c r="E2" s="36"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="34"/>
-      <c r="I2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="38"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="31"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="31"/>
+      <c r="A3" s="33"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="33"/>
       <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
@@ -2322,7 +2343,7 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" s="43" t="s">
+      <c r="A42" s="8" t="s">
         <v>13</v>
       </c>
       <c r="B42" s="8">
@@ -2353,7 +2374,7 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" s="43" t="s">
+      <c r="A43" s="8" t="s">
         <v>13</v>
       </c>
       <c r="B43" s="8">
@@ -2415,26 +2436,40 @@
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A45" s="8"/>
+      <c r="A45" s="8" t="s">
+        <v>58</v>
+      </c>
       <c r="B45" s="8"/>
       <c r="C45" s="8"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="8"/>
+      <c r="D45" s="8">
+        <v>202</v>
+      </c>
+      <c r="E45" s="8">
+        <v>209</v>
+      </c>
       <c r="F45" s="8">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="G45" s="8"/>
-      <c r="H45" s="8"/>
+        <v>7</v>
+      </c>
+      <c r="G45" s="8">
+        <v>806</v>
+      </c>
+      <c r="H45" s="8">
+        <v>820</v>
+      </c>
       <c r="I45" s="8">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A46" s="8"/>
+      <c r="A46" s="8" t="s">
+        <v>58</v>
+      </c>
       <c r="B46" s="8"/>
-      <c r="C46" s="8"/>
+      <c r="C46" s="8">
+        <v>-9</v>
+      </c>
       <c r="D46" s="8"/>
       <c r="E46" s="8"/>
       <c r="F46" s="8">
@@ -2468,7 +2503,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F87" sqref="F87"/>
+      <selection pane="bottomLeft" activeCell="H95" sqref="H95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2486,33 +2521,33 @@
       </c>
     </row>
     <row r="2" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="43" t="s">
         <v>16</v>
       </c>
       <c r="D2" s="18"/>
       <c r="E2" s="18"/>
       <c r="F2" s="18"/>
-      <c r="G2" s="40" t="s">
+      <c r="G2" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="H2" s="40"/>
+      <c r="H2" s="42"/>
       <c r="I2" s="19"/>
-      <c r="J2" s="40" t="s">
+      <c r="J2" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="K2" s="40"/>
+      <c r="K2" s="42"/>
       <c r="L2" s="19"/>
     </row>
     <row r="3" spans="1:12" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="38"/>
-      <c r="B3" s="39"/>
-      <c r="C3" s="42"/>
+      <c r="A3" s="40"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="44"/>
       <c r="D3" s="21" t="s">
         <v>46</v>
       </c>
@@ -4800,7 +4835,7 @@
       <c r="A69" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="B69" s="44">
+      <c r="B69" s="30">
         <v>-125</v>
       </c>
       <c r="C69" s="3">
@@ -4834,7 +4869,7 @@
       <c r="A70" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="B70" s="44">
+      <c r="B70" s="30">
         <v>-115</v>
       </c>
       <c r="C70" s="3">
@@ -4902,7 +4937,7 @@
       <c r="A72" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="B72" s="44">
+      <c r="B72" s="30">
         <v>-105</v>
       </c>
       <c r="C72" s="3">
@@ -4936,7 +4971,7 @@
       <c r="A73" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="B73" s="45">
+      <c r="B73" s="31">
         <v>-85</v>
       </c>
       <c r="C73" s="12">
@@ -5000,42 +5035,42 @@
         <v>-14</v>
       </c>
     </row>
-    <row r="75" spans="1:12" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:12" s="20" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A75" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="B75" s="47">
+      <c r="B75" s="3">
         <v>-125</v>
       </c>
       <c r="C75" s="3">
         <v>8.2699999999999996E-2</v>
       </c>
-      <c r="D75" s="47">
+      <c r="D75" s="3">
         <v>1079</v>
       </c>
-      <c r="E75" s="47">
+      <c r="E75" s="3">
         <v>20082</v>
       </c>
-      <c r="F75" s="47">
+      <c r="F75" s="3">
         <v>78</v>
       </c>
-      <c r="G75" s="46">
+      <c r="G75" s="24">
         <v>215</v>
       </c>
-      <c r="H75" s="46">
+      <c r="H75" s="24">
         <v>196</v>
       </c>
-      <c r="I75" s="46">
+      <c r="I75" s="24">
         <f t="shared" si="7"/>
         <v>-19</v>
       </c>
-      <c r="J75" s="46">
+      <c r="J75" s="24">
         <v>803</v>
       </c>
-      <c r="K75" s="46">
+      <c r="K75" s="24">
         <v>782</v>
       </c>
-      <c r="L75" s="46">
+      <c r="L75" s="24">
         <f t="shared" si="8"/>
         <v>-21</v>
       </c>
@@ -5080,42 +5115,42 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="77" spans="1:12" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:12" s="20" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A77" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="B77" s="47">
+      <c r="B77" s="3">
         <v>-125</v>
       </c>
-      <c r="C77" s="47">
+      <c r="C77" s="3">
         <v>8.3500000000000005E-2</v>
       </c>
-      <c r="D77" s="47">
+      <c r="D77" s="3">
         <v>1079</v>
       </c>
-      <c r="E77" s="47">
+      <c r="E77" s="3">
         <v>20082</v>
       </c>
-      <c r="F77" s="47">
+      <c r="F77" s="3">
         <v>78</v>
       </c>
-      <c r="G77" s="46">
+      <c r="G77" s="24">
         <v>214</v>
       </c>
-      <c r="H77" s="46">
+      <c r="H77" s="24">
         <v>188</v>
       </c>
-      <c r="I77" s="46">
+      <c r="I77" s="24">
         <f t="shared" si="11"/>
         <v>-26</v>
       </c>
-      <c r="J77" s="46">
+      <c r="J77" s="24">
         <v>820</v>
       </c>
-      <c r="K77" s="46">
+      <c r="K77" s="24">
         <v>799</v>
       </c>
-      <c r="L77" s="46">
+      <c r="L77" s="24">
         <f t="shared" si="12"/>
         <v>-21</v>
       </c>
@@ -5160,502 +5195,726 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="79" spans="1:12" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A79" s="46"/>
-      <c r="B79" s="47"/>
-      <c r="C79" s="47"/>
-      <c r="D79" s="47"/>
-      <c r="E79" s="47"/>
-      <c r="F79" s="47"/>
-      <c r="G79" s="46"/>
-      <c r="H79" s="46"/>
-      <c r="I79" s="46">
+    <row r="79" spans="1:12" s="20" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A79" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="B79" s="3">
+        <v>-85</v>
+      </c>
+      <c r="C79" s="3">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="D79" s="3"/>
+      <c r="E79" s="3"/>
+      <c r="F79" s="3"/>
+      <c r="G79" s="24">
+        <v>200</v>
+      </c>
+      <c r="H79" s="24">
+        <v>219</v>
+      </c>
+      <c r="I79" s="24">
+        <f t="shared" si="11"/>
+        <v>19</v>
+      </c>
+      <c r="J79" s="24">
+        <v>817</v>
+      </c>
+      <c r="K79" s="24">
+        <v>842</v>
+      </c>
+      <c r="L79" s="24">
+        <f t="shared" si="12"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" s="20" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A80" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="B80" s="3">
+        <v>-105</v>
+      </c>
+      <c r="C80" s="3">
+        <v>8.3500000000000005E-2</v>
+      </c>
+      <c r="D80" s="3"/>
+      <c r="E80" s="3"/>
+      <c r="F80" s="3"/>
+      <c r="G80" s="24">
+        <v>199</v>
+      </c>
+      <c r="H80" s="24">
+        <v>195</v>
+      </c>
+      <c r="I80" s="24">
+        <f t="shared" si="11"/>
+        <v>-4</v>
+      </c>
+      <c r="J80" s="24">
+        <v>799</v>
+      </c>
+      <c r="K80" s="24">
+        <v>805</v>
+      </c>
+      <c r="L80" s="24">
+        <f t="shared" si="12"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" s="26" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A81" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="B81" s="12">
+        <v>-100</v>
+      </c>
+      <c r="C81" s="12">
+        <v>8.2500000000000004E-2</v>
+      </c>
+      <c r="D81" s="12"/>
+      <c r="E81" s="12"/>
+      <c r="F81" s="12"/>
+      <c r="G81" s="25">
+        <v>205</v>
+      </c>
+      <c r="H81" s="25">
+        <v>207</v>
+      </c>
+      <c r="I81" s="25">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+      <c r="J81" s="25">
+        <v>799</v>
+      </c>
+      <c r="K81" s="25">
+        <v>805</v>
+      </c>
+      <c r="L81" s="25">
+        <f t="shared" si="12"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" s="20" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A82" s="45" t="s">
+        <v>56</v>
+      </c>
+      <c r="B82" s="3">
+        <v>-85</v>
+      </c>
+      <c r="C82" s="3">
+        <v>8.2500000000000004E-2</v>
+      </c>
+      <c r="D82" s="3"/>
+      <c r="E82" s="3"/>
+      <c r="F82" s="3"/>
+      <c r="G82" s="24">
+        <v>217</v>
+      </c>
+      <c r="H82" s="24">
+        <v>197</v>
+      </c>
+      <c r="I82" s="24">
+        <f t="shared" si="11"/>
+        <v>-20</v>
+      </c>
+      <c r="J82" s="24">
+        <v>817</v>
+      </c>
+      <c r="K82" s="24">
+        <v>785</v>
+      </c>
+      <c r="L82" s="24">
+        <f t="shared" si="12"/>
+        <v>-32</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" s="20" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A83" s="45" t="s">
+        <v>55</v>
+      </c>
+      <c r="B83" s="3">
+        <v>-70</v>
+      </c>
+      <c r="C83" s="3">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="D83" s="3"/>
+      <c r="E83" s="3"/>
+      <c r="F83" s="3"/>
+      <c r="G83" s="24">
+        <v>215</v>
+      </c>
+      <c r="H83" s="24">
+        <v>221</v>
+      </c>
+      <c r="I83" s="24">
+        <f t="shared" si="11"/>
+        <v>6</v>
+      </c>
+      <c r="J83" s="24">
+        <v>816</v>
+      </c>
+      <c r="K83" s="24">
+        <v>834</v>
+      </c>
+      <c r="L83" s="24">
+        <f t="shared" si="12"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" s="20" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A84" s="45" t="s">
+        <v>55</v>
+      </c>
+      <c r="B84" s="3">
+        <v>-70</v>
+      </c>
+      <c r="C84" s="3">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="D84" s="3"/>
+      <c r="E84" s="3"/>
+      <c r="F84" s="3"/>
+      <c r="G84" s="24">
+        <v>215</v>
+      </c>
+      <c r="H84" s="24">
+        <v>221</v>
+      </c>
+      <c r="I84" s="24">
+        <f t="shared" si="11"/>
+        <v>6</v>
+      </c>
+      <c r="J84" s="24">
+        <v>798</v>
+      </c>
+      <c r="K84" s="24">
+        <v>790</v>
+      </c>
+      <c r="L84" s="24">
+        <f t="shared" si="12"/>
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" s="20" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A85" s="45" t="s">
+        <v>55</v>
+      </c>
+      <c r="B85" s="3">
+        <v>-80</v>
+      </c>
+      <c r="C85" s="3">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="D85" s="3"/>
+      <c r="E85" s="3"/>
+      <c r="F85" s="3"/>
+      <c r="G85" s="24">
+        <v>198</v>
+      </c>
+      <c r="H85" s="24">
+        <v>197</v>
+      </c>
+      <c r="I85" s="24">
+        <f t="shared" si="11"/>
+        <v>-1</v>
+      </c>
+      <c r="J85" s="24">
+        <v>798</v>
+      </c>
+      <c r="K85" s="24">
+        <v>790</v>
+      </c>
+      <c r="L85" s="24">
+        <f t="shared" si="12"/>
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" s="26" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A86" s="46" t="s">
+        <v>55</v>
+      </c>
+      <c r="B86" s="12">
+        <v>-80</v>
+      </c>
+      <c r="C86" s="12">
+        <v>8.4500000000000006E-2</v>
+      </c>
+      <c r="D86" s="12"/>
+      <c r="E86" s="12"/>
+      <c r="F86" s="12"/>
+      <c r="G86" s="25">
+        <v>198</v>
+      </c>
+      <c r="H86" s="25">
+        <v>198</v>
+      </c>
+      <c r="I86" s="25">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="J79" s="46"/>
-      <c r="K79" s="46"/>
-      <c r="L79" s="46">
+      <c r="J86" s="25">
+        <v>798</v>
+      </c>
+      <c r="K86" s="25">
+        <v>803</v>
+      </c>
+      <c r="L86" s="25">
+        <f t="shared" si="12"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" s="20" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A87" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="B87" s="30">
+        <v>-80</v>
+      </c>
+      <c r="C87" s="3">
+        <v>8.4500000000000006E-2</v>
+      </c>
+      <c r="D87" s="3"/>
+      <c r="E87" s="3"/>
+      <c r="F87" s="3"/>
+      <c r="G87" s="24">
+        <v>195</v>
+      </c>
+      <c r="H87" s="24">
+        <v>198</v>
+      </c>
+      <c r="I87" s="24">
+        <f t="shared" si="11"/>
+        <v>3</v>
+      </c>
+      <c r="J87" s="24">
+        <v>793</v>
+      </c>
+      <c r="K87" s="24">
+        <v>804</v>
+      </c>
+      <c r="L87" s="24">
+        <f t="shared" si="12"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" s="26" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A88" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="B88" s="31">
+        <v>-80</v>
+      </c>
+      <c r="C88" s="12">
+        <v>8.4500000000000006E-2</v>
+      </c>
+      <c r="D88" s="12"/>
+      <c r="E88" s="12"/>
+      <c r="F88" s="12"/>
+      <c r="G88" s="25">
+        <v>198</v>
+      </c>
+      <c r="H88" s="25">
+        <v>197</v>
+      </c>
+      <c r="I88" s="25">
+        <f t="shared" si="11"/>
+        <v>-1</v>
+      </c>
+      <c r="J88" s="25">
+        <v>810</v>
+      </c>
+      <c r="K88" s="25">
+        <v>815</v>
+      </c>
+      <c r="L88" s="25">
+        <f t="shared" si="12"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" s="20" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A89" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="B89" s="3">
+        <v>-100</v>
+      </c>
+      <c r="C89" s="3">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="D89" s="3"/>
+      <c r="E89" s="3"/>
+      <c r="F89" s="3"/>
+      <c r="G89" s="24">
+        <v>211</v>
+      </c>
+      <c r="H89" s="24">
+        <v>219</v>
+      </c>
+      <c r="I89" s="24">
+        <f t="shared" si="11"/>
+        <v>8</v>
+      </c>
+      <c r="J89" s="24">
+        <v>807</v>
+      </c>
+      <c r="K89" s="24">
+        <v>822</v>
+      </c>
+      <c r="L89" s="24">
+        <f t="shared" si="12"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" s="20" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A90" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="B90" s="3">
+        <v>-100</v>
+      </c>
+      <c r="C90" s="3">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="D90" s="3"/>
+      <c r="E90" s="3"/>
+      <c r="F90" s="3"/>
+      <c r="G90" s="24">
+        <v>217</v>
+      </c>
+      <c r="H90" s="24">
+        <v>231</v>
+      </c>
+      <c r="I90" s="24">
+        <f t="shared" si="11"/>
+        <v>14</v>
+      </c>
+      <c r="J90" s="24">
+        <v>800</v>
+      </c>
+      <c r="K90" s="24">
+        <v>822</v>
+      </c>
+      <c r="L90" s="24">
+        <f t="shared" si="12"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" s="26" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A91" s="46" t="s">
+        <v>59</v>
+      </c>
+      <c r="B91" s="12">
+        <v>-110</v>
+      </c>
+      <c r="C91" s="12">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="D91" s="12"/>
+      <c r="E91" s="12"/>
+      <c r="F91" s="12"/>
+      <c r="G91" s="25">
+        <v>219</v>
+      </c>
+      <c r="H91" s="25">
+        <v>220</v>
+      </c>
+      <c r="I91" s="25">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="J91" s="25">
+        <v>807</v>
+      </c>
+      <c r="K91" s="25">
+        <v>806</v>
+      </c>
+      <c r="L91" s="25">
+        <f t="shared" si="12"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" s="20" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A92" s="45" t="s">
+        <v>60</v>
+      </c>
+      <c r="B92" s="3">
+        <v>-100</v>
+      </c>
+      <c r="C92" s="3">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="D92" s="3"/>
+      <c r="E92" s="3"/>
+      <c r="F92" s="3"/>
+      <c r="G92" s="24">
+        <v>199</v>
+      </c>
+      <c r="H92" s="24">
+        <v>160</v>
+      </c>
+      <c r="I92" s="24">
+        <f t="shared" si="11"/>
+        <v>-39</v>
+      </c>
+      <c r="J92" s="24">
+        <v>804</v>
+      </c>
+      <c r="K92" s="24">
+        <v>785</v>
+      </c>
+      <c r="L92" s="24">
+        <f t="shared" si="12"/>
+        <v>-19</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" s="20" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A93" s="45" t="s">
+        <v>60</v>
+      </c>
+      <c r="B93" s="3">
+        <v>-60</v>
+      </c>
+      <c r="C93" s="3">
+        <v>8.2500000000000004E-2</v>
+      </c>
+      <c r="D93" s="3"/>
+      <c r="E93" s="3"/>
+      <c r="F93" s="3"/>
+      <c r="G93" s="24">
+        <v>205</v>
+      </c>
+      <c r="H93" s="24">
+        <v>208</v>
+      </c>
+      <c r="I93" s="24">
+        <f t="shared" si="11"/>
+        <v>3</v>
+      </c>
+      <c r="J93" s="24">
+        <v>812</v>
+      </c>
+      <c r="K93" s="24">
+        <v>823</v>
+      </c>
+      <c r="L93" s="24">
+        <f t="shared" si="12"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" s="20" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A94" s="45" t="s">
+        <v>60</v>
+      </c>
+      <c r="B94" s="3">
+        <v>-60</v>
+      </c>
+      <c r="C94" s="3">
+        <v>8.1500000000000003E-2</v>
+      </c>
+      <c r="D94" s="3"/>
+      <c r="E94" s="3"/>
+      <c r="F94" s="3"/>
+      <c r="G94" s="24">
+        <v>212</v>
+      </c>
+      <c r="H94" s="24">
+        <v>210</v>
+      </c>
+      <c r="I94" s="24">
+        <f t="shared" si="11"/>
+        <v>-2</v>
+      </c>
+      <c r="J94" s="24">
+        <v>812</v>
+      </c>
+      <c r="K94" s="24">
+        <v>812</v>
+      </c>
+      <c r="L94" s="24">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:12" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A80" s="46"/>
-      <c r="B80" s="47"/>
-      <c r="C80" s="47"/>
-      <c r="D80" s="47"/>
-      <c r="E80" s="47"/>
-      <c r="F80" s="47"/>
-      <c r="G80" s="46"/>
-      <c r="H80" s="46"/>
-      <c r="I80" s="46">
+    <row r="95" spans="1:12" s="20" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A95" s="24"/>
+      <c r="B95" s="3"/>
+      <c r="C95" s="3"/>
+      <c r="D95" s="3"/>
+      <c r="E95" s="3"/>
+      <c r="F95" s="3"/>
+      <c r="G95" s="24"/>
+      <c r="H95" s="24"/>
+      <c r="I95" s="24">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="J80" s="46"/>
-      <c r="K80" s="46"/>
-      <c r="L80" s="46">
+      <c r="J95" s="24"/>
+      <c r="K95" s="24"/>
+      <c r="L95" s="24">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:12" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A81" s="46"/>
-      <c r="B81" s="47"/>
-      <c r="C81" s="47"/>
-      <c r="D81" s="47"/>
-      <c r="E81" s="47"/>
-      <c r="F81" s="47"/>
-      <c r="G81" s="46"/>
-      <c r="H81" s="46"/>
-      <c r="I81" s="46">
+    <row r="96" spans="1:12" s="20" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A96" s="24"/>
+      <c r="B96" s="3"/>
+      <c r="C96" s="3"/>
+      <c r="D96" s="3"/>
+      <c r="E96" s="3"/>
+      <c r="F96" s="3"/>
+      <c r="G96" s="24"/>
+      <c r="H96" s="24"/>
+      <c r="I96" s="24">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="J81" s="46"/>
-      <c r="K81" s="46"/>
-      <c r="L81" s="46">
+      <c r="J96" s="24"/>
+      <c r="K96" s="24"/>
+      <c r="L96" s="24">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:12" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A82" s="46"/>
-      <c r="B82" s="47"/>
-      <c r="C82" s="47"/>
-      <c r="D82" s="47"/>
-      <c r="E82" s="47"/>
-      <c r="F82" s="47"/>
-      <c r="G82" s="46"/>
-      <c r="H82" s="46"/>
-      <c r="I82" s="46">
+    <row r="97" spans="1:12" s="20" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A97" s="24"/>
+      <c r="B97" s="3"/>
+      <c r="C97" s="3"/>
+      <c r="D97" s="3"/>
+      <c r="E97" s="3"/>
+      <c r="F97" s="3"/>
+      <c r="G97" s="24"/>
+      <c r="H97" s="24"/>
+      <c r="I97" s="24">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="J82" s="46"/>
-      <c r="K82" s="46"/>
-      <c r="L82" s="46">
+      <c r="J97" s="24"/>
+      <c r="K97" s="24"/>
+      <c r="L97" s="24">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:12" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A83" s="46"/>
-      <c r="B83" s="47"/>
-      <c r="C83" s="47"/>
-      <c r="D83" s="47"/>
-      <c r="E83" s="47"/>
-      <c r="F83" s="47"/>
-      <c r="G83" s="46"/>
-      <c r="H83" s="46"/>
-      <c r="I83" s="46">
+    <row r="98" spans="1:12" s="20" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A98" s="24"/>
+      <c r="B98" s="3"/>
+      <c r="C98" s="3"/>
+      <c r="D98" s="3"/>
+      <c r="E98" s="3"/>
+      <c r="F98" s="3"/>
+      <c r="G98" s="24"/>
+      <c r="H98" s="24"/>
+      <c r="I98" s="24">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="J83" s="46"/>
-      <c r="K83" s="46"/>
-      <c r="L83" s="46">
+      <c r="J98" s="24"/>
+      <c r="K98" s="24"/>
+      <c r="L98" s="24">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:12" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A84" s="46"/>
-      <c r="B84" s="47"/>
-      <c r="C84" s="47"/>
-      <c r="D84" s="47"/>
-      <c r="E84" s="47"/>
-      <c r="F84" s="47"/>
-      <c r="G84" s="46"/>
-      <c r="H84" s="46"/>
-      <c r="I84" s="46">
+    <row r="99" spans="1:12" s="20" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A99" s="24"/>
+      <c r="B99" s="3"/>
+      <c r="C99" s="3"/>
+      <c r="D99" s="3"/>
+      <c r="E99" s="3"/>
+      <c r="F99" s="3"/>
+      <c r="G99" s="24"/>
+      <c r="H99" s="24"/>
+      <c r="I99" s="24">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="J84" s="46"/>
-      <c r="K84" s="46"/>
-      <c r="L84" s="46">
+      <c r="J99" s="24"/>
+      <c r="K99" s="24"/>
+      <c r="L99" s="24">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:12" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A85" s="46"/>
-      <c r="B85" s="47"/>
-      <c r="C85" s="47"/>
-      <c r="D85" s="47"/>
-      <c r="E85" s="47"/>
-      <c r="F85" s="47"/>
-      <c r="G85" s="46"/>
-      <c r="H85" s="46"/>
-      <c r="I85" s="46">
+    <row r="100" spans="1:12" s="20" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A100" s="24"/>
+      <c r="B100" s="3"/>
+      <c r="C100" s="3"/>
+      <c r="D100" s="3"/>
+      <c r="E100" s="3"/>
+      <c r="F100" s="3"/>
+      <c r="G100" s="24"/>
+      <c r="H100" s="24"/>
+      <c r="I100" s="24">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="J85" s="46"/>
-      <c r="K85" s="46"/>
-      <c r="L85" s="46">
+      <c r="J100" s="24"/>
+      <c r="K100" s="24"/>
+      <c r="L100" s="24">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:12" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A86" s="46"/>
-      <c r="B86" s="47"/>
-      <c r="C86" s="47"/>
-      <c r="D86" s="47"/>
-      <c r="E86" s="47"/>
-      <c r="F86" s="47"/>
-      <c r="G86" s="46"/>
-      <c r="H86" s="46"/>
-      <c r="I86" s="46">
+    <row r="101" spans="1:12" s="20" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A101" s="24"/>
+      <c r="B101" s="3"/>
+      <c r="C101" s="3"/>
+      <c r="D101" s="3"/>
+      <c r="E101" s="3"/>
+      <c r="F101" s="3"/>
+      <c r="G101" s="24"/>
+      <c r="H101" s="24"/>
+      <c r="I101" s="24">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="J86" s="46"/>
-      <c r="K86" s="46"/>
-      <c r="L86" s="46">
+      <c r="J101" s="24"/>
+      <c r="K101" s="24"/>
+      <c r="L101" s="24">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:12" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A87" s="46"/>
-      <c r="B87" s="47"/>
-      <c r="C87" s="47"/>
-      <c r="D87" s="47"/>
-      <c r="E87" s="47"/>
-      <c r="F87" s="47"/>
-      <c r="G87" s="46"/>
-      <c r="H87" s="46"/>
-      <c r="I87" s="46">
+    <row r="102" spans="1:12" s="20" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A102" s="24"/>
+      <c r="B102" s="3"/>
+      <c r="C102" s="3"/>
+      <c r="D102" s="3"/>
+      <c r="E102" s="3"/>
+      <c r="F102" s="3"/>
+      <c r="G102" s="24"/>
+      <c r="H102" s="24"/>
+      <c r="I102" s="24">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="J87" s="46"/>
-      <c r="K87" s="46"/>
-      <c r="L87" s="46">
+      <c r="J102" s="24"/>
+      <c r="K102" s="24"/>
+      <c r="L102" s="24">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:12" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A88" s="46"/>
-      <c r="B88" s="47"/>
-      <c r="C88" s="47"/>
-      <c r="D88" s="47"/>
-      <c r="E88" s="47"/>
-      <c r="F88" s="47"/>
-      <c r="G88" s="46"/>
-      <c r="H88" s="46"/>
-      <c r="I88" s="46">
+    <row r="103" spans="1:12" s="20" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A103" s="24"/>
+      <c r="B103" s="3"/>
+      <c r="C103" s="3"/>
+      <c r="D103" s="3"/>
+      <c r="E103" s="3"/>
+      <c r="F103" s="3"/>
+      <c r="G103" s="24"/>
+      <c r="H103" s="24"/>
+      <c r="I103" s="24">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="J88" s="46"/>
-      <c r="K88" s="46"/>
-      <c r="L88" s="46">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:12" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A89" s="46"/>
-      <c r="B89" s="47"/>
-      <c r="C89" s="47"/>
-      <c r="D89" s="47"/>
-      <c r="E89" s="47"/>
-      <c r="F89" s="47"/>
-      <c r="G89" s="46"/>
-      <c r="H89" s="46"/>
-      <c r="I89" s="46">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="J89" s="46"/>
-      <c r="K89" s="46"/>
-      <c r="L89" s="46">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:12" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A90" s="46"/>
-      <c r="B90" s="47"/>
-      <c r="C90" s="47"/>
-      <c r="D90" s="47"/>
-      <c r="E90" s="47"/>
-      <c r="F90" s="47"/>
-      <c r="G90" s="46"/>
-      <c r="H90" s="46"/>
-      <c r="I90" s="46">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="J90" s="46"/>
-      <c r="K90" s="46"/>
-      <c r="L90" s="46">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:12" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A91" s="46"/>
-      <c r="B91" s="47"/>
-      <c r="C91" s="47"/>
-      <c r="D91" s="47"/>
-      <c r="E91" s="47"/>
-      <c r="F91" s="47"/>
-      <c r="G91" s="46"/>
-      <c r="H91" s="46"/>
-      <c r="I91" s="46">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="J91" s="46"/>
-      <c r="K91" s="46"/>
-      <c r="L91" s="46">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:12" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A92" s="46"/>
-      <c r="B92" s="47"/>
-      <c r="C92" s="47"/>
-      <c r="D92" s="47"/>
-      <c r="E92" s="47"/>
-      <c r="F92" s="47"/>
-      <c r="G92" s="46"/>
-      <c r="H92" s="46"/>
-      <c r="I92" s="46">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="J92" s="46"/>
-      <c r="K92" s="46"/>
-      <c r="L92" s="46">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:12" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A93" s="46"/>
-      <c r="B93" s="47"/>
-      <c r="C93" s="47"/>
-      <c r="D93" s="47"/>
-      <c r="E93" s="47"/>
-      <c r="F93" s="47"/>
-      <c r="G93" s="46"/>
-      <c r="H93" s="46"/>
-      <c r="I93" s="46">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="J93" s="46"/>
-      <c r="K93" s="46"/>
-      <c r="L93" s="46">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:12" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A94" s="46"/>
-      <c r="B94" s="47"/>
-      <c r="C94" s="47"/>
-      <c r="D94" s="47"/>
-      <c r="E94" s="47"/>
-      <c r="F94" s="47"/>
-      <c r="G94" s="46"/>
-      <c r="H94" s="46"/>
-      <c r="I94" s="46">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="J94" s="46"/>
-      <c r="K94" s="46"/>
-      <c r="L94" s="46">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:12" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A95" s="46"/>
-      <c r="B95" s="47"/>
-      <c r="C95" s="47"/>
-      <c r="D95" s="47"/>
-      <c r="E95" s="47"/>
-      <c r="F95" s="47"/>
-      <c r="G95" s="46"/>
-      <c r="H95" s="46"/>
-      <c r="I95" s="46">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="J95" s="46"/>
-      <c r="K95" s="46"/>
-      <c r="L95" s="46">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:12" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A96" s="46"/>
-      <c r="B96" s="47"/>
-      <c r="C96" s="47"/>
-      <c r="D96" s="47"/>
-      <c r="E96" s="47"/>
-      <c r="F96" s="47"/>
-      <c r="G96" s="46"/>
-      <c r="H96" s="46"/>
-      <c r="I96" s="46">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="J96" s="46"/>
-      <c r="K96" s="46"/>
-      <c r="L96" s="46">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:12" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A97" s="46"/>
-      <c r="B97" s="47"/>
-      <c r="C97" s="47"/>
-      <c r="D97" s="47"/>
-      <c r="E97" s="47"/>
-      <c r="F97" s="47"/>
-      <c r="G97" s="46"/>
-      <c r="H97" s="46"/>
-      <c r="I97" s="46">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="J97" s="46"/>
-      <c r="K97" s="46"/>
-      <c r="L97" s="46">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:12" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A98" s="46"/>
-      <c r="B98" s="47"/>
-      <c r="C98" s="47"/>
-      <c r="D98" s="47"/>
-      <c r="E98" s="47"/>
-      <c r="F98" s="47"/>
-      <c r="G98" s="46"/>
-      <c r="H98" s="46"/>
-      <c r="I98" s="46">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="J98" s="46"/>
-      <c r="K98" s="46"/>
-      <c r="L98" s="46">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:12" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A99" s="46"/>
-      <c r="B99" s="47"/>
-      <c r="C99" s="47"/>
-      <c r="D99" s="47"/>
-      <c r="E99" s="47"/>
-      <c r="F99" s="47"/>
-      <c r="G99" s="46"/>
-      <c r="H99" s="46"/>
-      <c r="I99" s="46">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="J99" s="46"/>
-      <c r="K99" s="46"/>
-      <c r="L99" s="46">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:12" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A100" s="46"/>
-      <c r="B100" s="47"/>
-      <c r="C100" s="47"/>
-      <c r="D100" s="47"/>
-      <c r="E100" s="47"/>
-      <c r="F100" s="47"/>
-      <c r="G100" s="46"/>
-      <c r="H100" s="46"/>
-      <c r="I100" s="46">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="J100" s="46"/>
-      <c r="K100" s="46"/>
-      <c r="L100" s="46">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:12" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A101" s="46"/>
-      <c r="B101" s="47"/>
-      <c r="C101" s="47"/>
-      <c r="D101" s="47"/>
-      <c r="E101" s="47"/>
-      <c r="F101" s="47"/>
-      <c r="G101" s="46"/>
-      <c r="H101" s="46"/>
-      <c r="I101" s="46">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="J101" s="46"/>
-      <c r="K101" s="46"/>
-      <c r="L101" s="46">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:12" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A102" s="46"/>
-      <c r="B102" s="47"/>
-      <c r="C102" s="47"/>
-      <c r="D102" s="47"/>
-      <c r="E102" s="47"/>
-      <c r="F102" s="47"/>
-      <c r="G102" s="46"/>
-      <c r="H102" s="46"/>
-      <c r="I102" s="46">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="J102" s="46"/>
-      <c r="K102" s="46"/>
-      <c r="L102" s="46">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="1:12" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A103" s="46"/>
-      <c r="B103" s="47"/>
-      <c r="C103" s="47"/>
-      <c r="D103" s="47"/>
-      <c r="E103" s="47"/>
-      <c r="F103" s="47"/>
-      <c r="G103" s="46"/>
-      <c r="H103" s="46"/>
-      <c r="I103" s="46">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="J103" s="46"/>
-      <c r="K103" s="46"/>
-      <c r="L103" s="46">
+      <c r="J103" s="24"/>
+      <c r="K103" s="24"/>
+      <c r="L103" s="24">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>

</xml_diff>